<commit_message>
Repository name change and directory restructuring
</commit_message>
<xml_diff>
--- a/Teaching_assignments.xlsx
+++ b/Teaching_assignments.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t xml:space="preserve">Programming</t>
   </si>
@@ -127,6 +127,9 @@
     <t xml:space="preserve">Time Management</t>
   </si>
   <si>
+    <t xml:space="preserve">Scala</t>
+  </si>
+  <si>
     <t xml:space="preserve">Symfony</t>
   </si>
   <si>
@@ -139,6 +142,9 @@
     <t xml:space="preserve">BDD (Behaviour Driven Development)</t>
   </si>
   <si>
+    <t xml:space="preserve">Erlang</t>
+  </si>
+  <si>
     <t xml:space="preserve">CakePHP</t>
   </si>
   <si>
@@ -151,6 +157,9 @@
     <t xml:space="preserve">TDD (Test Driven Development)</t>
   </si>
   <si>
+    <t xml:space="preserve">Clojure</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yii2</t>
   </si>
   <si>
@@ -163,6 +172,9 @@
     <t xml:space="preserve">Micro Services</t>
   </si>
   <si>
+    <t xml:space="preserve">Go</t>
+  </si>
+  <si>
     <t xml:space="preserve">Code Igniter</t>
   </si>
   <si>
@@ -172,6 +184,9 @@
     <t xml:space="preserve">Unit Testing</t>
   </si>
   <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
     <t xml:space="preserve">VueJS</t>
   </si>
   <si>
@@ -181,6 +196,9 @@
     <t xml:space="preserve">RESTful API Designing and Development</t>
   </si>
   <si>
+    <t xml:space="preserve">Rust</t>
+  </si>
+  <si>
     <t xml:space="preserve">React</t>
   </si>
   <si>
@@ -188,6 +206,9 @@
   </si>
   <si>
     <t xml:space="preserve">Android App</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elixir (On Erlang VM)</t>
   </si>
   <si>
     <t xml:space="preserve">NodeJS</t>
@@ -229,6 +250,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -250,6 +272,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -323,18 +346,18 @@
   <dimension ref="B1:G17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9438775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.9234693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.0561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,115 +478,136 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>35</v>
+      </c>
       <c r="D7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="D8" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="D9" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>50</v>
+      </c>
       <c r="D10" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>54</v>
+      </c>
       <c r="D11" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>58</v>
+      </c>
       <c r="D12" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="D13" s="0" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="0" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="0" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>